<commit_message>
Modulação do código e alteração na validação de senha
</commit_message>
<xml_diff>
--- a/usuarios.xlsx
+++ b/usuarios.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -481,7 +481,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>10/10/2010</t>
+          <t>18/11/2004</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -491,37 +491,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Hip-Hop, Grunge</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>usuario@gmail.com</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>usuario</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>30/03/2001</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Feminino</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Indie Pop, Indie Rock</t>
+          <t>Pop, Alternativa</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Adicionando mensagens de status de criação de conta ao terminal
</commit_message>
<xml_diff>
--- a/usuarios.xlsx
+++ b/usuarios.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -495,6 +495,186 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>usuarioteste@gmail.com</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>usuarioteste</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>10/12/2004</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Prefiro não informar</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Alternativa, Experimental</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>aaaaaaaa@gmail.com</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>aaaaaaa</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>18/11/2004</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Feminino</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Pop, Alternativa</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>fgh@gmail.com</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>qwsdefrf</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>11/11/2011</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Feminino</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Grunge</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>asdf@gmail.com</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>ad</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>11/11/2011</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Feminino</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Pop</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>aaaaaa@gmail.com</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>11/11/2004</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Feminino</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Rock</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>ghjk@gmail.com</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>sedrfgt</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>11/11/2004</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Feminino</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Hip-Hop</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>